<commit_message>
Fix sales family items discount account code
</commit_message>
<xml_diff>
--- a/Saudi/roomOccupancy.xlsx
+++ b/Saudi/roomOccupancy.xlsx
@@ -19,34 +19,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Room Status</t>
+    <t>RoomsAvailable </t>
   </si>
   <si>
-    <t>Counter</t>
+    <t>RoomsOccupied</t>
   </si>
   <si>
-    <t>DI</t>
-  </si>
-  <si>
-    <t>IP</t>
-  </si>
-  <si>
-    <t>CL</t>
-  </si>
-  <si>
-    <t>OO</t>
-  </si>
-  <si>
-    <t>OS</t>
+    <t>RoomsOnMaintenance </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,25 +170,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="3"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -389,7 +363,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -501,6 +475,21 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
       </bottom>
       <diagonal/>
     </border>
@@ -549,20 +538,23 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -888,85 +880,52 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="9" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="13.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5">
-        <v>312</v>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>194</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>3</v>
+      <c r="B3" s="6">
+        <v>266</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5">
-        <v>37</v>
+      <c r="C3" s="6">
+        <v>12</v>
       </c>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5">
-        <v>111</v>
-      </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5">
-        <v>12</v>
-      </c>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5">
-        <v>5</v>
-      </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>